<commit_message>
ETS2 question, swing state
</commit_message>
<xml_diff>
--- a/questionnaire/specificities.xlsx
+++ b/questionnaire/specificities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="11880" tabRatio="687" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19220" windowHeight="11880" tabRatio="687" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="705">
   <si>
     <t>France</t>
   </si>
@@ -2119,6 +2119,36 @@
   </si>
   <si>
     <t>Formula: ((e/E)*(f/a)*A/F)*R/a (this is an approximation, for the full computation, see code_global/map_GCS_incidence.R)</t>
+  </si>
+  <si>
+    <t>Mt CO2 emissions</t>
+  </si>
+  <si>
+    <t>Price (€/tCO2)</t>
+  </si>
+  <si>
+    <t>2019 road transport + household fuel emissions share of EU's</t>
+  </si>
+  <si>
+    <t>EU27 &gt;14 population from World Bank (2023) https://databank.worldbank.org/source/population-estimates-and-projections</t>
+  </si>
+  <si>
+    <t>Pop &gt;14 2015</t>
+  </si>
+  <si>
+    <t>Pop &gt;14 2030</t>
+  </si>
+  <si>
+    <t>ETS2 revenues per adult &gt;14 (in €/month, at €45/tCO2 for 800MtCO2)</t>
+  </si>
+  <si>
+    <t>Eurostat's env_air_gge, summing CO2 emissions from fuel combustion in road transport, commercial and institutional sector, and by households</t>
+  </si>
+  <si>
+    <t>EU's objective is 2,2Gt in 2030 (https://climateactiontracker.org/countries/eu/targets/), of which 40-45% should be in ETS2 (hence 900Mt-1Gt).</t>
+  </si>
+  <si>
+    <t>Q123 revenues pc ETS2 (EU: €105 per year)</t>
   </si>
 </sst>
 </file>
@@ -2301,7 +2331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2452,6 +2482,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2733,19 +2768,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P183"/>
+  <dimension ref="A1:P186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="60.08984375" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2773,9 +2808,7 @@
       <c r="I1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" t="s">
-        <v>61</v>
-      </c>
+      <c r="J1" s="81"/>
       <c r="K1" t="s">
         <v>32</v>
       </c>
@@ -2783,7 +2816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>39</v>
       </c>
@@ -2813,11 +2846,14 @@
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
       <c r="N2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
@@ -2845,7 +2881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
@@ -2873,7 +2909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -2889,7 +2925,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>358</v>
       </c>
@@ -2924,7 +2960,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
@@ -2953,7 +2989,7 @@
         <v>285.30725980380089</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>42</v>
       </c>
@@ -2985,7 +3021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -3022,7 +3058,7 @@
         <v>23.777393803164124</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>54</v>
       </c>
@@ -3056,7 +3092,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>30</v>
       </c>
@@ -3085,7 +3121,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>31</v>
       </c>
@@ -3121,9 +3157,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>17</v>
+        <v>699</v>
       </c>
       <c r="B13" s="4">
         <v>52684007</v>
@@ -3155,9 +3191,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
-        <v>18</v>
+        <v>700</v>
       </c>
       <c r="B14" s="4">
         <v>56464893</v>
@@ -3185,11 +3221,14 @@
         <f>SUM(B14:F14)</f>
         <v>234328547</v>
       </c>
+      <c r="J14" s="2">
+        <v>383210000</v>
+      </c>
       <c r="M14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>684</v>
       </c>
@@ -3220,1023 +3259,1106 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G16" s="78"/>
+      <c r="K16" s="18" t="s">
+        <v>695</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>696</v>
+      </c>
+      <c r="M16" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="B17" s="84">
+        <f>$K$17*1000000*$L$17*B18/B14</f>
+        <v>109.68530799528163</v>
+      </c>
+      <c r="C17" s="84">
+        <f t="shared" ref="C17:J17" si="3">$K$17*1000000*$L$17*C18/C14</f>
+        <v>130.37348091980942</v>
+      </c>
+      <c r="D17" s="84">
+        <f t="shared" si="3"/>
+        <v>89.435739829717861</v>
+      </c>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84">
+        <f t="shared" si="3"/>
+        <v>105.68617729182432</v>
+      </c>
+      <c r="K17" s="18">
+        <v>900</v>
+      </c>
+      <c r="L17" s="18">
+        <v>45</v>
+      </c>
+      <c r="M17" s="81" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="B18" s="3">
+        <f>(123073+40352+21637)/(783587+301450+125130)</f>
+        <v>0.15292269579322523</v>
+      </c>
+      <c r="C18" s="3">
+        <f>(157437+89449+29711)/(783587+301450+125130)</f>
+        <v>0.22856101678528665</v>
+      </c>
+      <c r="D18" s="3">
+        <f>(83548+14157+10546)/(783587+301450+125130)</f>
+        <v>8.9451290606998871E-2</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="78"/>
+      <c r="J18" s="81">
+        <v>1</v>
+      </c>
+      <c r="M18" s="81" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="78"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="11">
-        <f t="shared" ref="B17:G17" si="3">B21/B20</f>
+      <c r="B20" s="11">
+        <f t="shared" ref="B20:G23" si="4">B24/B23</f>
         <v>1.6804869000780116E-2</v>
       </c>
-      <c r="C17" s="11">
-        <f t="shared" si="3"/>
+      <c r="C20" s="11">
+        <f t="shared" si="4"/>
         <v>2.4285946906251236E-2</v>
       </c>
-      <c r="D17" s="11">
-        <f t="shared" si="3"/>
+      <c r="D20" s="11">
+        <f t="shared" si="4"/>
         <v>8.4503315316459028E-3</v>
       </c>
-      <c r="E17" s="11">
-        <f t="shared" si="3"/>
+      <c r="E20" s="11">
+        <f t="shared" si="4"/>
         <v>2.182641984567564E-2</v>
       </c>
-      <c r="F17" s="11">
-        <f t="shared" si="3"/>
+      <c r="F20" s="11">
+        <f t="shared" si="4"/>
         <v>2.7832459188770545E-2</v>
       </c>
-      <c r="G17" s="11">
-        <f t="shared" si="3"/>
+      <c r="G20" s="3"/>
+      <c r="J20" s="81"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="B21" s="11">
+        <f>B24/B22</f>
+        <v>2.8652771056078725E-2</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" ref="C21:G24" si="5">C24/C22</f>
+        <v>3.7067064609916489E-2</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="5"/>
+        <v>1.4677280378829026E-2</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11">
+        <f t="shared" si="5"/>
+        <v>3.8580944213005321E-2</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="B22" s="11">
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.13320000000000001</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0.1144</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11">
+        <v>0.12740000000000001</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="M22" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0.15260000000000001</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.20330000000000001</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0.19869999999999999</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0.19109999999999999</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0.17660000000000001</v>
+      </c>
+      <c r="G23" s="11">
+        <f t="shared" si="4"/>
         <v>4.5731003235390304E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="B18" s="11">
-        <f>B21/B19</f>
-        <v>2.8652771056078725E-2</v>
-      </c>
-      <c r="C18" s="11">
-        <f t="shared" ref="C18:G18" si="4">C21/C19</f>
-        <v>3.7067064609916489E-2</v>
-      </c>
-      <c r="D18" s="11">
-        <f t="shared" si="4"/>
-        <v>1.4677280378829026E-2</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11">
-        <f t="shared" si="4"/>
-        <v>3.8580944213005321E-2</v>
-      </c>
-      <c r="G18" s="11">
-        <f t="shared" si="4"/>
+      <c r="M23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="3">
+        <f>B7/B25</f>
+        <v>2.5644230095190458E-3</v>
+      </c>
+      <c r="C24" s="3">
+        <f>C7/C25</f>
+        <v>4.9373330060408765E-3</v>
+      </c>
+      <c r="D24" s="3">
+        <f>D7/D25</f>
+        <v>1.6790808753380407E-3</v>
+      </c>
+      <c r="E24" s="3">
+        <f>E7/E25</f>
+        <v>4.1710288325086144E-3</v>
+      </c>
+      <c r="F24" s="3">
+        <f>F7/F25</f>
+        <v>4.9152122927368785E-3</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="5"/>
         <v>6.5196117592019917E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>428</v>
-      </c>
-      <c r="B19" s="11">
-        <v>8.9499999999999996E-2</v>
-      </c>
-      <c r="C19" s="11">
-        <v>0.13320000000000001</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0.1144</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11">
-        <v>0.12740000000000001</v>
-      </c>
-      <c r="G19" s="11">
+      <c r="M24" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25">
+        <v>2937</v>
+      </c>
+      <c r="C25">
+        <v>4223</v>
+      </c>
+      <c r="D25">
+        <v>1425</v>
+      </c>
+      <c r="E25">
+        <v>813</v>
+      </c>
+      <c r="F25">
+        <v>3187</v>
+      </c>
+      <c r="G25" s="11">
         <v>0.1903</v>
       </c>
-      <c r="M19" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="11">
-        <v>0.15260000000000001</v>
-      </c>
-      <c r="C20" s="11">
-        <v>0.20330000000000001</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0.19869999999999999</v>
-      </c>
-      <c r="E20" s="11">
-        <v>0.19109999999999999</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0.17660000000000001</v>
-      </c>
-      <c r="G20" s="11">
+      <c r="M25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
+        <v>431</v>
+      </c>
+      <c r="B26" s="41">
+        <v>175</v>
+      </c>
+      <c r="C26" s="41">
+        <v>249</v>
+      </c>
+      <c r="D26" s="41">
+        <v>132</v>
+      </c>
+      <c r="E26" s="36"/>
+      <c r="F26" s="41">
+        <v>178</v>
+      </c>
+      <c r="G26" s="11">
         <v>0.27129999999999999</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M26" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>95</v>
+      </c>
+      <c r="C27">
+        <v>112</v>
+      </c>
+      <c r="D27">
+        <v>83</v>
+      </c>
+      <c r="E27">
+        <v>152</v>
+      </c>
+      <c r="F27">
+        <v>88</v>
+      </c>
+      <c r="G27" s="3">
+        <f>G7/G28</f>
+        <v>1.2406821177761389E-2</v>
+      </c>
+      <c r="M27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" ref="B21:G21" si="5">B7/B22</f>
-        <v>2.5644230095190458E-3</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" si="5"/>
-        <v>4.9373330060408765E-3</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="5"/>
-        <v>1.6790808753380407E-3</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="5"/>
-        <v>4.1710288325086144E-3</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="5"/>
-        <v>4.9152122927368785E-3</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="5"/>
-        <v>1.2406821177761389E-2</v>
-      </c>
-      <c r="M21" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22">
-        <v>2937</v>
-      </c>
-      <c r="C22">
-        <v>4223</v>
-      </c>
-      <c r="D22">
-        <v>1425</v>
-      </c>
-      <c r="E22">
-        <v>813</v>
-      </c>
-      <c r="F22">
-        <v>3187</v>
-      </c>
-      <c r="G22">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28">
         <v>22996</v>
       </c>
-      <c r="M22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>431</v>
-      </c>
-      <c r="B23" s="41">
-        <v>175</v>
-      </c>
-      <c r="C23" s="41">
-        <v>249</v>
-      </c>
-      <c r="D23" s="41">
-        <v>132</v>
-      </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="41">
-        <v>178</v>
-      </c>
-      <c r="G23" s="41">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="C29">
+        <v>83.1</v>
+      </c>
+      <c r="D29">
+        <v>47.1</v>
+      </c>
+      <c r="E29">
+        <v>8.6</v>
+      </c>
+      <c r="F29">
+        <v>66.8</v>
+      </c>
+      <c r="G29" s="41">
         <v>479</v>
-      </c>
-      <c r="M23" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24">
-        <v>95</v>
-      </c>
-      <c r="C24">
-        <v>112</v>
-      </c>
-      <c r="D24">
-        <v>83</v>
-      </c>
-      <c r="E24">
-        <v>152</v>
-      </c>
-      <c r="F24">
-        <v>88</v>
-      </c>
-      <c r="G24">
-        <v>172</v>
-      </c>
-      <c r="M24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26">
-        <v>67.400000000000006</v>
-      </c>
-      <c r="C26">
-        <v>83.1</v>
-      </c>
-      <c r="D26">
-        <v>47.1</v>
-      </c>
-      <c r="E26">
-        <v>8.6</v>
-      </c>
-      <c r="F26">
-        <v>66.8</v>
-      </c>
-      <c r="G26">
-        <v>328.3</v>
-      </c>
-      <c r="H26">
-        <f>SUM(B26+C26+D26+F26)</f>
-        <v>264.39999999999998</v>
-      </c>
-      <c r="I26">
-        <f>H26+E26</f>
-        <v>273</v>
-      </c>
-      <c r="J26">
-        <v>446.8</v>
-      </c>
-      <c r="M26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="4">
-        <v>51.7</v>
-      </c>
-      <c r="C27" s="2">
-        <v>69.400000000000006</v>
-      </c>
-      <c r="D27" s="2">
-        <v>38.5</v>
-      </c>
-      <c r="E27" s="2">
-        <v>7.11</v>
-      </c>
-      <c r="F27" s="2">
-        <v>53.1</v>
-      </c>
-      <c r="G27" s="4">
-        <v>257</v>
-      </c>
-      <c r="H27" s="2">
-        <f>SUM(B27:F27)</f>
-        <v>219.81000000000003</v>
-      </c>
-      <c r="I27" s="2">
-        <f>H27+E27</f>
-        <v>226.92000000000004</v>
-      </c>
-      <c r="M27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28">
-        <v>27012</v>
-      </c>
-      <c r="C28">
-        <v>25039</v>
-      </c>
-      <c r="D28">
-        <v>17656</v>
-      </c>
-      <c r="E28">
-        <v>23603</v>
-      </c>
-      <c r="F28">
-        <v>19798</v>
-      </c>
-      <c r="G28">
-        <v>24858</v>
-      </c>
-      <c r="M28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="2">
-        <v>469000</v>
-      </c>
-      <c r="C29" s="2">
-        <f>C28*C26</f>
-        <v>2080740.9</v>
-      </c>
-      <c r="D29" s="2">
-        <f>D28*D26</f>
-        <v>831597.6</v>
-      </c>
-      <c r="E29" s="2">
-        <f>E28*E26</f>
-        <v>202985.8</v>
-      </c>
-      <c r="F29" s="2">
-        <f>F28*F26</f>
-        <v>1322506.3999999999</v>
-      </c>
-      <c r="G29" s="2">
-        <v>4496000</v>
       </c>
       <c r="H29">
         <f>SUM(B29+C29+D29+F29)</f>
-        <v>4703844.9000000004</v>
+        <v>264.39999999999998</v>
       </c>
       <c r="I29">
         <f>H29+E29</f>
+        <v>273</v>
+      </c>
+      <c r="M29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="4">
+        <v>51.7</v>
+      </c>
+      <c r="C30" s="2">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="D30" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>7.11</v>
+      </c>
+      <c r="F30" s="2">
+        <v>53.1</v>
+      </c>
+      <c r="G30">
+        <v>172</v>
+      </c>
+      <c r="H30" s="2">
+        <f>SUM(B30:F30)</f>
+        <v>219.81000000000003</v>
+      </c>
+      <c r="I30" s="2">
+        <f>H30+E30</f>
+        <v>226.92000000000004</v>
+      </c>
+      <c r="J30">
+        <v>446.8</v>
+      </c>
+      <c r="M30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>27012</v>
+      </c>
+      <c r="C31">
+        <v>25039</v>
+      </c>
+      <c r="D31">
+        <v>17656</v>
+      </c>
+      <c r="E31">
+        <v>23603</v>
+      </c>
+      <c r="F31">
+        <v>19798</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="M31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2">
+        <v>469000</v>
+      </c>
+      <c r="C32" s="2">
+        <f>C31*C29</f>
+        <v>2080740.9</v>
+      </c>
+      <c r="D32" s="2">
+        <f>D31*D29</f>
+        <v>831597.6</v>
+      </c>
+      <c r="E32" s="2">
+        <f>E31*E29</f>
+        <v>202985.8</v>
+      </c>
+      <c r="F32" s="2">
+        <f>F31*F29</f>
+        <v>1322506.3999999999</v>
+      </c>
+      <c r="G32">
+        <v>328.3</v>
+      </c>
+      <c r="H32">
+        <f>SUM(B32+C32+D32+F32)</f>
+        <v>4703844.9000000004</v>
+      </c>
+      <c r="I32">
+        <f>H32+E32</f>
         <v>4906830.7</v>
       </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="M29" t="s">
+      <c r="K32" s="2"/>
+      <c r="M32" t="s">
         <v>33</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B30">
+      <c r="B33">
         <v>3079</v>
       </c>
-      <c r="G30">
+      <c r="G33" s="4">
+        <v>257</v>
+      </c>
+      <c r="J33" s="2"/>
+      <c r="M33" t="s">
+        <v>33</v>
+      </c>
+      <c r="N33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3">
+        <f>B33/B32</f>
+        <v>6.5650319829424304E-3</v>
+      </c>
+      <c r="C34" s="3" t="e">
+        <f>#REF!/C32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D34" s="3" t="e">
+        <f>#REF!/D32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E34" s="3" t="e">
+        <f>#REF!/E32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F34" s="3" t="e">
+        <f>#REF!/F32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G34">
+        <v>24858</v>
+      </c>
+      <c r="H34" s="3" t="e">
+        <f>#REF!/H32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I34" s="3" t="e">
+        <f>#REF!/I32</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="3">
+        <f>B4/B3</f>
+        <v>7.9422382671480145E-3</v>
+      </c>
+      <c r="C35" s="3">
+        <f>C4/C3</f>
+        <v>1.3333333333333332E-2</v>
+      </c>
+      <c r="D35" s="3">
+        <f>D4/D3</f>
+        <v>4.9881235154394295E-3</v>
+      </c>
+      <c r="E35" s="3">
+        <f>E4/E3</f>
+        <v>1.3414634146341463E-2</v>
+      </c>
+      <c r="F35" s="3">
+        <f>F4/F3</f>
+        <v>1.7199017199017199E-2</v>
+      </c>
+      <c r="G35" s="2">
+        <v>4496000</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="3" t="e">
+        <f>(#REF!*#REF!+B33)/B32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C36" s="3" t="e">
+        <f>(#REF!*#REF!+#REF!)/C32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D36" s="3" t="e">
+        <f>(#REF!*#REF!+#REF!)/D32</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F36" s="11">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="G36">
         <v>44100</v>
       </c>
-      <c r="M30" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3">
-        <f>B30/B29</f>
-        <v>6.5650319829424304E-3</v>
-      </c>
-      <c r="C31" s="3" t="e">
-        <f>#REF!/C29</f>
+      <c r="H36" s="3" t="e">
+        <f>(#REF!*#REF!+#REF!)/H32</f>
         <v>#REF!</v>
       </c>
-      <c r="D31" s="3" t="e">
-        <f>#REF!/D29</f>
+      <c r="I36" s="3" t="e">
+        <f>(#REF!*#REF!+#REF!)/I32</f>
         <v>#REF!</v>
       </c>
-      <c r="E31" s="3" t="e">
-        <f>#REF!/E29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F31" s="3" t="e">
-        <f>#REF!/F29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G31" s="3">
-        <f>G30/G29</f>
+      <c r="M36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="2">
+        <f>B6*B30*12/1000</f>
+        <v>7.1975864434768866</v>
+      </c>
+      <c r="C37" s="2">
+        <f>C6*C30*12/1000</f>
+        <v>21.032191795712752</v>
+      </c>
+      <c r="D37" s="2">
+        <f>D6*D30*12/1000</f>
+        <v>2.3499636357967666</v>
+      </c>
+      <c r="E37" s="2">
+        <f>E6*E30*12/1000</f>
+        <v>3.1934225422910951</v>
+      </c>
+      <c r="F37" s="2">
+        <f>F6*F30*12/1000</f>
+        <v>14.853569673860253</v>
+      </c>
+      <c r="G37" s="3">
+        <f>G36/G35</f>
         <v>9.8087188612099637E-3</v>
       </c>
-      <c r="H31" s="3" t="e">
-        <f>#REF!/H29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I31" s="3" t="e">
-        <f>#REF!/I29</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="3">
-        <f t="shared" ref="B32:G32" si="6">B4/B3</f>
-        <v>7.9422382671480145E-3</v>
-      </c>
-      <c r="C32" s="3">
-        <f t="shared" si="6"/>
-        <v>1.3333333333333332E-2</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="6"/>
-        <v>4.9881235154394295E-3</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="6"/>
-        <v>1.3414634146341463E-2</v>
-      </c>
-      <c r="F32" s="3">
-        <f t="shared" si="6"/>
-        <v>1.7199017199017199E-2</v>
-      </c>
-      <c r="G32" s="3">
-        <f t="shared" si="6"/>
-        <v>4.1884816753926706E-3</v>
-      </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="3" t="e">
-        <f>(#REF!*#REF!+B30)/B29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C33" s="3" t="e">
-        <f>(#REF!*#REF!+#REF!)/C29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D33" s="3" t="e">
-        <f>(#REF!*#REF!+#REF!)/D29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F33" s="11">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="H33" s="3" t="e">
-        <f>(#REF!*#REF!+#REF!)/H29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I33" s="3" t="e">
-        <f>(#REF!*#REF!+#REF!)/I29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="2">
-        <f t="shared" ref="B34:G34" si="7">B6*B27*12/1000</f>
-        <v>7.1975864434768866</v>
-      </c>
-      <c r="C34" s="2">
-        <f t="shared" si="7"/>
-        <v>21.032191795712752</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="7"/>
-        <v>2.3499636357967666</v>
-      </c>
-      <c r="E34" s="2">
-        <f t="shared" si="7"/>
-        <v>3.1934225422910951</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" si="7"/>
-        <v>14.853569673860253</v>
-      </c>
-      <c r="G34" s="2">
-        <f t="shared" si="7"/>
-        <v>264.04020802872463</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A38" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B38" s="2">
         <f>Constants!$B$6*B9*12*B14/10^9</f>
         <v>10.333402166480258</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C38" s="2">
         <f>Constants!$B$6*C9*12*C14/10^9</f>
         <v>25.143552870628557</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D38" s="2">
         <f>Constants!$B$6*D9*12*D14/10^9</f>
         <v>4.1054218110057965</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E38" s="2">
         <f>Constants!$B$6*E9*12*E14/10^9</f>
         <v>3.9671629464069529</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F38" s="2">
         <f>Constants!$B$6*F9*12*F14/10^9</f>
         <v>19.299485959819044</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G38" s="3">
+        <f>G4/G3</f>
+        <v>4.1884816753926706E-3</v>
+      </c>
+      <c r="H38" s="2">
+        <f>Constants!$B$6*H9*12*H14/10^9</f>
+        <v>62.849025754340616</v>
+      </c>
+      <c r="I38" s="2">
+        <f>Constants!$B$6*I9*12*I14/10^9</f>
+        <v>62.849025754340616</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="2">
+        <f>2000*B30/$H$30</f>
+        <v>470.40625995177646</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" ref="C39:F39" si="6">2000*C30/$H$30</f>
+        <v>631.4544379236612</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="6"/>
+        <v>350.30253400664208</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2">
+        <f t="shared" si="6"/>
+        <v>483.14453391565434</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A40" s="14"/>
+      <c r="G40" s="2">
+        <f>G6*G33*12/1000</f>
+        <v>264.04020802872463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" s="14"/>
+      <c r="G41" s="2">
         <f>Constants!$B$6*G9*12*G14/10^9</f>
         <v>322.14084632849483</v>
       </c>
-      <c r="H35" s="2">
-        <f>Constants!$B$6*H9*12*H14/10^9</f>
-        <v>62.849025754340616</v>
-      </c>
-      <c r="I35" s="2">
-        <f>Constants!$B$6*I9*12*I14/10^9</f>
-        <v>62.849025754340616</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="2">
-        <f>2000*B27/$H$27</f>
-        <v>470.40625995177646</v>
-      </c>
-      <c r="C36" s="2">
-        <f t="shared" ref="C36:F36" si="8">2000*C27/$H$27</f>
-        <v>631.4544379236612</v>
-      </c>
-      <c r="D36" s="2">
-        <f t="shared" si="8"/>
-        <v>350.30253400664208</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2">
-        <f t="shared" si="8"/>
-        <v>483.14453391565434</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="14"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="14"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="14"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="14"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="14"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="14"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="14"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="14"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="14"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="14"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="14"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="14"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="14"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="14"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="14"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="14"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="14"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="14"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="14"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="14"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="14"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="14"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="14"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="14"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="14"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="14"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="14"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="14"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="14"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="14"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="14"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="14"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="14"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="14"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="14"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="14"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="14"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="14"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="14"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="14"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="14"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="14"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="14"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="14"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="14"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="14"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="14"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="14"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="14"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="14"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="14"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="14"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="14"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="14"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="14"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="14"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="14"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="14"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="14"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="14"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="14"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="14"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="14"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="14"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="14"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="14"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="14"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="14"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="14"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="14"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="14"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="14"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="14"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="14"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="14"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="14"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="14"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="14"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="14"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="14"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="14"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="14"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="14"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="14"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="14"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="14"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="14"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="14"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="14"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="14"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="14"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="14"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="14"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="14"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="14"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="14"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="14"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="14"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="14"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="14"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="14"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="14"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="14"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="14"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="14"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="14"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="14"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="14"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="14"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="14"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="14"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="14"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="14"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="14"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" s="14"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" s="14"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" s="14"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="14"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="14"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" s="14"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" s="14"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" s="14"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" s="14"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" s="14"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" s="14"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" s="14"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" s="14"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" s="14"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" s="14"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" s="14"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" s="14"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" s="14"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" s="14"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" s="14"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" s="14"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" s="14"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" s="14"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" s="14"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" s="14"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="14"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" s="14"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" s="14"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" s="14"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" s="14"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4246,25 +4368,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" customWidth="1"/>
-    <col min="6" max="6" width="40.5703125" customWidth="1"/>
-    <col min="7" max="7" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.54296875" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" customWidth="1"/>
+    <col min="5" max="5" width="46.1796875" customWidth="1"/>
+    <col min="6" max="6" width="40.54296875" customWidth="1"/>
+    <col min="7" max="7" width="1.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>330</v>
       </c>
@@ -4284,15 +4406,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>334</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>342</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
       <c r="E2" t="s">
         <v>335</v>
       </c>
@@ -4300,7 +4422,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>336</v>
       </c>
@@ -4320,21 +4442,21 @@
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>339</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="82" t="s">
         <v>340</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
       <c r="F4" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>397</v>
       </c>
@@ -4354,7 +4476,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>445</v>
       </c>
@@ -4374,7 +4496,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>449</v>
       </c>
@@ -4394,7 +4516,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>450</v>
       </c>
@@ -4411,7 +4533,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>437</v>
       </c>
@@ -4431,7 +4553,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>347</v>
       </c>
@@ -4451,21 +4573,21 @@
         <v>349</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>350</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="82" t="s">
         <v>351</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
       <c r="F11" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>574</v>
       </c>
@@ -4485,7 +4607,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>354</v>
       </c>
@@ -4505,7 +4627,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>417</v>
       </c>
@@ -4525,33 +4647,33 @@
         <v>364</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>366</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="82" t="s">
         <v>367</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>368</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="82" t="s">
         <v>418</v>
       </c>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
       <c r="F16" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>370</v>
       </c>
@@ -4571,7 +4693,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>398</v>
       </c>
@@ -4591,21 +4713,21 @@
         <v>377</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>438</v>
       </c>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="82" t="s">
         <v>378</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
       <c r="F19" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>410</v>
       </c>
@@ -4625,7 +4747,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>383</v>
       </c>
@@ -4645,21 +4767,21 @@
         <v>384</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>385</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="82" t="s">
         <v>386</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
       <c r="F22" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>388</v>
       </c>
@@ -4679,21 +4801,21 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>389</v>
       </c>
-      <c r="B24" s="80" t="s">
+      <c r="B24" s="82" t="s">
         <v>348</v>
       </c>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
       <c r="F24" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>394</v>
       </c>
@@ -4713,308 +4835,323 @@
         <v>395</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>391</v>
       </c>
-      <c r="B26" s="80" t="s">
+      <c r="B26" s="82" t="s">
         <v>393</v>
       </c>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
       <c r="F26" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="81" t="s">
+        <v>704</v>
+      </c>
+      <c r="B27" s="80">
+        <v>110</v>
+      </c>
+      <c r="C27" s="80">
+        <v>130</v>
+      </c>
+      <c r="D27" s="80">
+        <v>90</v>
+      </c>
+      <c r="E27" s="80"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>409</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>407</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>403</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>402</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>400</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>439</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>408</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>404</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>405</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>401</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>414</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>416</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>411</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>412</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>415</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>413</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H30" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>600</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>594</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>595</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>596</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>597</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>599</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>584</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>601</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>602</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>603</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>604</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>605</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>585</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>588</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>589</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>590</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>591</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>593</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H33" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>586</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B34" s="83" t="s">
         <v>625</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" t="s">
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" t="s">
         <v>623</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>474</v>
       </c>
-      <c r="B34" s="79"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" t="s">
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F36" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F37" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F38" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F38" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F41" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F42" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F42" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F43" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F43" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F44" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F44" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F45" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F45" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F46" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F46" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F47" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F48" s="70" t="s">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F49" s="70" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="70" t="s">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F50" s="70" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="70" t="s">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F51" s="70" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F51" s="70" t="s">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F52" s="70" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F52" s="70" t="s">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F53" s="70" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F53" s="70" t="s">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F54" s="70" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F55" s="70" t="s">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F56" s="70" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F56" s="70" t="s">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F57" s="70" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F57" s="70" t="s">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F58" s="70" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F58" s="70" t="s">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F59" s="70" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F59" s="70" t="s">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F60" s="70" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="70" t="s">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F61" s="70" t="s">
         <v>498</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B34:E34"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5030,42 +5167,42 @@
       <selection pane="bottomLeft" activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" customWidth="1"/>
+    <col min="9" max="9" width="6.26953125" customWidth="1"/>
+    <col min="10" max="10" width="5.7265625" customWidth="1"/>
+    <col min="11" max="11" width="5.453125" customWidth="1"/>
     <col min="12" max="12" width="5" customWidth="1"/>
-    <col min="13" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" customWidth="1"/>
-    <col min="16" max="18" width="5.42578125" customWidth="1"/>
+    <col min="13" max="14" width="5.453125" customWidth="1"/>
+    <col min="15" max="15" width="6.1796875" customWidth="1"/>
+    <col min="16" max="18" width="5.453125" customWidth="1"/>
     <col min="19" max="19" width="5" customWidth="1"/>
-    <col min="20" max="20" width="5.28515625" customWidth="1"/>
-    <col min="21" max="22" width="5.42578125" customWidth="1"/>
+    <col min="20" max="20" width="5.26953125" customWidth="1"/>
+    <col min="21" max="22" width="5.453125" customWidth="1"/>
     <col min="23" max="23" width="4" customWidth="1"/>
-    <col min="24" max="24" width="4.5703125" customWidth="1"/>
-    <col min="25" max="26" width="3.85546875" customWidth="1"/>
-    <col min="27" max="29" width="5.42578125" customWidth="1"/>
-    <col min="30" max="30" width="8.5703125" customWidth="1"/>
-    <col min="31" max="31" width="8.42578125" customWidth="1"/>
+    <col min="24" max="24" width="4.54296875" customWidth="1"/>
+    <col min="25" max="26" width="3.81640625" customWidth="1"/>
+    <col min="27" max="29" width="5.453125" customWidth="1"/>
+    <col min="30" max="30" width="8.54296875" customWidth="1"/>
+    <col min="31" max="31" width="8.453125" customWidth="1"/>
     <col min="32" max="32" width="9" customWidth="1"/>
-    <col min="33" max="33" width="8.28515625" customWidth="1"/>
-    <col min="34" max="34" width="8.42578125" customWidth="1"/>
-    <col min="35" max="36" width="8.28515625" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" customWidth="1"/>
-    <col min="40" max="40" width="8.85546875" customWidth="1"/>
-    <col min="41" max="41" width="7.85546875" customWidth="1"/>
+    <col min="33" max="33" width="8.26953125" customWidth="1"/>
+    <col min="34" max="34" width="8.453125" customWidth="1"/>
+    <col min="35" max="36" width="8.26953125" customWidth="1"/>
+    <col min="37" max="37" width="9.1796875" customWidth="1"/>
+    <col min="40" max="40" width="8.81640625" customWidth="1"/>
+    <col min="41" max="41" width="7.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -5193,7 +5330,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>86</v>
       </c>
@@ -5304,7 +5441,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>87</v>
       </c>
@@ -5418,7 +5555,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>88</v>
       </c>
@@ -5526,7 +5663,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
@@ -5643,7 +5780,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>615</v>
       </c>
@@ -5765,7 +5902,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -5881,7 +6018,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -5989,7 +6126,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>616</v>
       </c>
@@ -6104,7 +6241,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>587</v>
       </c>
@@ -6215,7 +6352,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="U11" t="s">
         <v>685</v>
@@ -6233,7 +6370,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="12" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>304</v>
       </c>
@@ -6259,7 +6396,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>86</v>
       </c>
@@ -6346,7 +6483,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
         <v>87</v>
       </c>
@@ -6433,7 +6570,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>88</v>
       </c>
@@ -6520,7 +6657,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:43" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>3</v>
       </c>
@@ -6604,7 +6741,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>305</v>
       </c>
@@ -6692,7 +6829,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>306</v>
       </c>
@@ -6780,7 +6917,7 @@
         <v>291.3</v>
       </c>
     </row>
-    <row r="19" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>307</v>
       </c>
@@ -6868,7 +7005,7 @@
         <v>128.881</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>308</v>
       </c>
@@ -6939,7 +7076,7 @@
         <v>112.1</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="AD21" t="s">
         <v>5</v>
       </c>
@@ -7027,16 +7164,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -7047,7 +7184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -7058,7 +7195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -7069,7 +7206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -7080,7 +7217,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -7088,7 +7225,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -7096,7 +7233,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>359</v>
       </c>
@@ -7104,22 +7241,22 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -7137,12 +7274,12 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>75</v>
       </c>
@@ -7186,7 +7323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -7236,7 +7373,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -7286,7 +7423,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -7336,7 +7473,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7383,7 +7520,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -7430,7 +7567,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7477,12 +7614,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="O9" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>75</v>
       </c>
@@ -7532,7 +7669,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -7580,7 +7717,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -7628,7 +7765,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -7676,7 +7813,7 @@
         <v>4900</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -7724,7 +7861,7 @@
         <v>6700</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -7765,7 +7902,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -7824,18 +7961,18 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="34.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" customWidth="1"/>
+    <col min="4" max="4" width="30.453125" customWidth="1"/>
+    <col min="5" max="5" width="35.26953125" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="34.54296875" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -7861,7 +7998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -7890,7 +8027,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -7919,7 +8056,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -7948,7 +8085,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7977,7 +8114,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8006,7 +8143,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>324</v>
       </c>
@@ -8049,17 +8186,17 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" customWidth="1"/>
-    <col min="6" max="6" width="50.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" customWidth="1"/>
+    <col min="2" max="2" width="40.54296875" customWidth="1"/>
+    <col min="3" max="3" width="47.7265625" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" customWidth="1"/>
+    <col min="5" max="5" width="46.54296875" customWidth="1"/>
+    <col min="6" max="6" width="50.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>196</v>
       </c>
@@ -8080,7 +8217,7 @@
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>175</v>
       </c>
@@ -8101,7 +8238,7 @@
       </c>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -8112,7 +8249,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>161</v>
       </c>
@@ -8133,7 +8270,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>5</v>
       </c>
@@ -8154,7 +8291,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>167</v>
       </c>
@@ -8175,7 +8312,7 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>165</v>
       </c>
@@ -8196,7 +8333,7 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>164</v>
       </c>
@@ -8217,7 +8354,7 @@
       </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>9</v>
       </c>
@@ -8228,7 +8365,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>166</v>
       </c>
@@ -8251,7 +8388,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>163</v>
       </c>
@@ -8274,7 +8411,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>162</v>
       </c>
@@ -8297,7 +8434,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>568</v>
       </c>
@@ -8318,7 +8455,7 @@
       </c>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>567</v>
       </c>
@@ -8339,7 +8476,7 @@
       </c>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>15</v>
       </c>
@@ -8350,7 +8487,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>547</v>
       </c>
@@ -8373,7 +8510,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>533</v>
       </c>
@@ -8396,7 +8533,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>534</v>
       </c>
@@ -8419,7 +8556,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>535</v>
       </c>
@@ -8442,7 +8579,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>536</v>
       </c>
@@ -8465,7 +8602,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="8">
         <v>21</v>
       </c>
@@ -8488,7 +8625,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>551</v>
       </c>
@@ -8511,7 +8648,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>537</v>
       </c>
@@ -8534,7 +8671,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>538</v>
       </c>
@@ -8557,7 +8694,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="8">
         <v>25</v>
       </c>
@@ -8580,7 +8717,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="8">
         <v>26</v>
       </c>
@@ -8595,7 +8732,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>550</v>
       </c>
@@ -8618,7 +8755,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>539</v>
       </c>
@@ -8641,7 +8778,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>540</v>
       </c>
@@ -8664,7 +8801,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>541</v>
       </c>
@@ -8687,7 +8824,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="8">
         <v>31</v>
       </c>
@@ -8710,7 +8847,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>549</v>
       </c>
@@ -8733,7 +8870,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="76" t="s">
         <v>532</v>
       </c>
@@ -8756,7 +8893,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="76" t="s">
         <v>542</v>
       </c>
@@ -8779,7 +8916,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="8">
         <v>35</v>
       </c>
@@ -8802,7 +8939,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="8">
         <v>36</v>
       </c>
@@ -8817,7 +8954,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>548</v>
       </c>
@@ -8840,7 +8977,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>543</v>
       </c>
@@ -8863,7 +9000,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>544</v>
       </c>
@@ -8886,7 +9023,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>545</v>
       </c>
@@ -8909,7 +9046,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>546</v>
       </c>
@@ -8932,7 +9069,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="8">
         <v>42</v>
       </c>
@@ -8953,7 +9090,7 @@
       </c>
       <c r="G42" s="75"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="8">
         <v>43</v>
       </c>
@@ -8971,7 +9108,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="8">
         <v>44</v>
       </c>
@@ -8987,7 +9124,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="8">
         <v>45</v>
       </c>
@@ -9003,7 +9140,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -9015,7 +9152,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -9027,7 +9164,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -9041,13 +9178,13 @@
         <v>648</v>
       </c>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E49" s="77" t="s">
         <v>476</v>
       </c>
       <c r="G49" s="77"/>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E50" s="77" t="s">
         <v>477</v>
       </c>
@@ -9058,7 +9195,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E51" s="77" t="s">
         <v>478</v>
       </c>
@@ -9069,7 +9206,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E52" s="77" t="s">
         <v>479</v>
       </c>
@@ -9080,7 +9217,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E53" s="77" t="s">
         <v>480</v>
       </c>
@@ -9091,7 +9228,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E54" s="77"/>
       <c r="F54" s="8" t="s">
         <v>485</v>
@@ -9100,7 +9237,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E55" s="77" t="s">
         <v>481</v>
       </c>
@@ -9111,12 +9248,12 @@
         <v>654</v>
       </c>
     </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E56" s="77" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E57" s="77" t="s">
         <v>483</v>
       </c>
@@ -9127,7 +9264,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E58" s="77" t="s">
         <v>484</v>
       </c>
@@ -9138,7 +9275,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E59" s="77" t="s">
         <v>485</v>
       </c>
@@ -9149,7 +9286,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E60" s="77" t="s">
         <v>486</v>
       </c>
@@ -9160,7 +9297,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:7" x14ac:dyDescent="0.35">
       <c r="F61" t="s">
         <v>491</v>
       </c>
@@ -9168,7 +9305,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:7" x14ac:dyDescent="0.35">
       <c r="F62" t="s">
         <v>492</v>
       </c>
@@ -9176,7 +9313,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:7" x14ac:dyDescent="0.35">
       <c r="F64" t="s">
         <v>493</v>
       </c>
@@ -9184,7 +9321,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="65" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F65" t="s">
         <v>494</v>
       </c>
@@ -9192,7 +9329,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="66" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F66" t="s">
         <v>664</v>
       </c>
@@ -9200,7 +9337,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="67" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F67" t="s">
         <v>683</v>
       </c>
@@ -9208,7 +9345,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="68" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F68" t="s">
         <v>497</v>
       </c>
@@ -9216,7 +9353,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="69" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F69" t="s">
         <v>498</v>
       </c>
@@ -9238,32 +9375,32 @@
       <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="4" width="7" customWidth="1"/>
-    <col min="5" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" customWidth="1"/>
-    <col min="20" max="20" width="7.140625" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" customWidth="1"/>
-    <col min="22" max="22" width="8.42578125" customWidth="1"/>
+    <col min="5" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" customWidth="1"/>
+    <col min="9" max="9" width="6.81640625" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" customWidth="1"/>
+    <col min="13" max="13" width="8.1796875" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" customWidth="1"/>
+    <col min="17" max="17" width="6.7265625" customWidth="1"/>
+    <col min="18" max="18" width="11.453125" customWidth="1"/>
+    <col min="19" max="19" width="8.54296875" customWidth="1"/>
+    <col min="20" max="20" width="7.1796875" customWidth="1"/>
+    <col min="21" max="21" width="9.54296875" customWidth="1"/>
+    <col min="22" max="22" width="8.453125" customWidth="1"/>
     <col min="23" max="23" width="8" customWidth="1"/>
     <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" customWidth="1"/>
-    <col min="27" max="27" width="8.28515625" customWidth="1"/>
+    <col min="26" max="26" width="13.1796875" customWidth="1"/>
+    <col min="27" max="27" width="8.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>196</v>
       </c>
@@ -9345,7 +9482,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>87</v>
       </c>
@@ -9444,7 +9581,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>88</v>
       </c>
@@ -9543,7 +9680,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>86</v>
       </c>
@@ -9642,7 +9779,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>202</v>
       </c>
@@ -9741,7 +9878,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" s="34" t="s">
         <v>203</v>
       </c>
@@ -9835,7 +9972,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>205</v>
       </c>
@@ -9929,7 +10066,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" s="37"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -9964,7 +10101,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>3</v>
       </c>
@@ -10012,7 +10149,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>5</v>
       </c>
@@ -10054,7 +10191,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" s="37"/>
       <c r="B11" s="26"/>
       <c r="D11" s="26"/>
@@ -10070,7 +10207,7 @@
       <c r="V11" s="32"/>
       <c r="W11" s="5"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -10121,7 +10258,7 @@
         <v>260000</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>211</v>
       </c>
@@ -10174,7 +10311,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>212</v>
       </c>
@@ -10227,7 +10364,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>213</v>
       </c>
@@ -10280,7 +10417,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -10333,7 +10470,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -10386,7 +10523,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>216</v>
       </c>
@@ -10439,7 +10576,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>217</v>
       </c>
@@ -10492,7 +10629,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
         <v>251</v>
       </c>
@@ -10510,7 +10647,7 @@
       <c r="V20" s="32"/>
       <c r="W20" s="5"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="E21" t="s">
         <v>253</v>
       </c>
@@ -10529,7 +10666,7 @@
       <c r="V21" s="32"/>
       <c r="W21" s="5"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
         <v>254</v>
       </c>
@@ -10550,7 +10687,7 @@
       <c r="V22" s="32"/>
       <c r="W22" s="5"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="23" t="s">
         <v>218</v>
       </c>
@@ -10598,7 +10735,7 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="23" t="s">
         <v>219</v>
       </c>
@@ -10646,7 +10783,7 @@
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>220</v>
       </c>
@@ -10694,7 +10831,7 @@
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="23" t="s">
         <v>221</v>
       </c>
@@ -10742,7 +10879,7 @@
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>222</v>
       </c>
@@ -10790,7 +10927,7 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="23" t="s">
         <v>223</v>
       </c>
@@ -10838,7 +10975,7 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="23" t="s">
         <v>224</v>
       </c>
@@ -10886,7 +11023,7 @@
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>225</v>
       </c>
@@ -10934,7 +11071,7 @@
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>226</v>
       </c>
@@ -10982,7 +11119,7 @@
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>227</v>
       </c>
@@ -11030,7 +11167,7 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
         <v>228</v>
       </c>
@@ -11078,7 +11215,7 @@
       <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
         <v>229</v>
       </c>
@@ -11126,7 +11263,7 @@
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>230</v>
       </c>
@@ -11174,7 +11311,7 @@
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
         <v>231</v>
       </c>
@@ -11222,7 +11359,7 @@
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>232</v>
       </c>
@@ -11270,7 +11407,7 @@
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>233</v>
       </c>
@@ -11318,7 +11455,7 @@
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="23" t="s">
         <v>234</v>
       </c>
@@ -11366,7 +11503,7 @@
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="23" t="s">
         <v>235</v>
       </c>
@@ -11428,15 +11565,15 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" customWidth="1"/>
+    <col min="18" max="18" width="11.453125" customWidth="1"/>
     <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="33" max="33" width="11.42578125" customWidth="1"/>
+    <col min="33" max="33" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="14" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="14" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -11535,7 +11672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -11646,7 +11783,7 @@
         <v>10.333402166480258</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -11755,7 +11892,7 @@
         <v>25.143552870628557</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -11864,7 +12001,7 @@
         <v>4.1054218110057965</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -11965,7 +12102,7 @@
         <v>3.9671629464069529</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -12069,7 +12206,7 @@
         <v>19.299485959819044</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -12172,7 +12309,7 @@
         <v>322.14084632849483</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -12231,7 +12368,7 @@
         <v>62.849025754340616</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -12290,7 +12427,7 @@
         <v>62.849025754340616</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -12302,7 +12439,7 @@
       </c>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -12315,7 +12452,7 @@
       </c>
       <c r="AB11" s="2"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -12380,7 +12517,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>57</v>
       </c>
@@ -12394,7 +12531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B15" s="18" t="s">
         <v>64</v>
       </c>
@@ -12402,7 +12539,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
median gain over GDP, measures reflection
</commit_message>
<xml_diff>
--- a/questionnaire/specificities.xlsx
+++ b/questionnaire/specificities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19220" windowHeight="11880" tabRatio="687" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="11880" tabRatio="687" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Figures" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="726">
   <si>
     <t>France</t>
   </si>
@@ -2200,6 +2200,18 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>South &amp; South-East Asia</t>
+  </si>
+  <si>
+    <t>East Asia</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>North America</t>
   </si>
 </sst>
 </file>
@@ -2382,7 +2394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2549,6 +2561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2843,12 +2856,12 @@
       <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.1796875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="60.140625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -2884,7 +2897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>39</v>
       </c>
@@ -2921,7 +2934,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
@@ -2949,7 +2962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
@@ -2977,7 +2990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -2993,7 +3006,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>357</v>
       </c>
@@ -3028,7 +3041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
@@ -3057,7 +3070,7 @@
         <v>285.30725980380089</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>42</v>
       </c>
@@ -3089,7 +3102,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -3126,7 +3139,7 @@
         <v>23.777393803164124</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>54</v>
       </c>
@@ -3160,7 +3173,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>30</v>
       </c>
@@ -3189,7 +3202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>31</v>
       </c>
@@ -3225,7 +3238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>693</v>
       </c>
@@ -3259,7 +3272,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>694</v>
       </c>
@@ -3296,7 +3309,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>678</v>
       </c>
@@ -3327,7 +3340,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -3345,7 +3358,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" s="81" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>695</v>
       </c>
@@ -3380,7 +3393,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>691</v>
       </c>
@@ -3406,7 +3419,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -3415,7 +3428,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="78"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>51</v>
       </c>
@@ -3442,7 +3455,7 @@
       <c r="G20" s="3"/>
       <c r="J20" s="81"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>425</v>
       </c>
@@ -3465,7 +3478,7 @@
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>423</v>
       </c>
@@ -3487,7 +3500,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>49</v>
       </c>
@@ -3514,7 +3527,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>69</v>
       </c>
@@ -3546,7 +3559,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>48</v>
       </c>
@@ -3572,7 +3585,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>426</v>
       </c>
@@ -3596,7 +3609,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>50</v>
       </c>
@@ -3623,7 +3636,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>71</v>
       </c>
@@ -3636,7 +3649,7 @@
         <v>22996</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>70</v>
       </c>
@@ -3670,7 +3683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>53</v>
       </c>
@@ -3707,7 +3720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>10</v>
       </c>
@@ -3731,7 +3744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>11</v>
       </c>
@@ -3773,7 +3786,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>35</v>
       </c>
@@ -3791,7 +3804,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>7</v>
       </c>
@@ -3827,7 +3840,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>39</v>
       </c>
@@ -3857,7 +3870,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>15</v>
       </c>
@@ -3891,7 +3904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>55</v>
       </c>
@@ -3920,7 +3933,7 @@
         <v>9.8087188612099637E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>20</v>
       </c>
@@ -3957,7 +3970,7 @@
         <v>62.849025754340616</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>105</v>
       </c>
@@ -3979,453 +3992,453 @@
         <v>483.14453391565434</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="G40" s="2">
         <f>G6*G33*12/1000</f>
         <v>264.04020802872463</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="G41" s="2">
         <f>Constants!$B$6*G9*12*G14/10^9</f>
         <v>322.14084632849483</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="14"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="14"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="14"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="14"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="14"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="14"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="14"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="14"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="14"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="14"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="14"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="14"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="14"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="14"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="14"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="14"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="14"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="14"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="14"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="14"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="14"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="14"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="14"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="14"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="14"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="14"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="14"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="14"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="14"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="14"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="14"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="14"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="14"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="14"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="14"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="14"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="14"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="14"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="14"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="14"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="14"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="14"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="14"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="14"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="14"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="14"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="14"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="14"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="14"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="14"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="14"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="14"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="14"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="14"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="14"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="14"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="14"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="14"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="14"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="14"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="14"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="14"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="14"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="14"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="14"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="14"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="14"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="14"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="14"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="14"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="14"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="14"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="14"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="14"/>
     </row>
   </sheetData>
@@ -4443,18 +4456,18 @@
       <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="46.54296875" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" customWidth="1"/>
-    <col min="5" max="5" width="46.1796875" customWidth="1"/>
-    <col min="6" max="6" width="40.54296875" customWidth="1"/>
-    <col min="7" max="7" width="1.26953125" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+    <col min="6" max="6" width="40.5703125" customWidth="1"/>
+    <col min="7" max="7" width="1.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>329</v>
       </c>
@@ -4474,15 +4487,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>333</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="93" t="s">
         <v>341</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
       <c r="E2" t="s">
         <v>334</v>
       </c>
@@ -4490,7 +4503,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>335</v>
       </c>
@@ -4510,21 +4523,21 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>338</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="93" t="s">
         <v>339</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
       <c r="F4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>393</v>
       </c>
@@ -4544,7 +4557,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>440</v>
       </c>
@@ -4564,7 +4577,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>444</v>
       </c>
@@ -4584,7 +4597,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>445</v>
       </c>
@@ -4601,7 +4614,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>432</v>
       </c>
@@ -4621,7 +4634,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>346</v>
       </c>
@@ -4641,21 +4654,21 @@
         <v>348</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>349</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="93" t="s">
         <v>350</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
       <c r="F11" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>569</v>
       </c>
@@ -4675,7 +4688,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>353</v>
       </c>
@@ -4695,7 +4708,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>413</v>
       </c>
@@ -4715,19 +4728,19 @@
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>365</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="93" t="s">
         <v>366</v>
       </c>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-    </row>
-    <row r="16" spans="1:6" s="90" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93"/>
+    </row>
+    <row r="16" spans="1:6" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="90" t="s">
         <v>718</v>
       </c>
@@ -4747,7 +4760,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>367</v>
       </c>
@@ -4767,7 +4780,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>394</v>
       </c>
@@ -4787,21 +4800,21 @@
         <v>374</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>433</v>
       </c>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="93" t="s">
         <v>375</v>
       </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
       <c r="F19" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>406</v>
       </c>
@@ -4821,7 +4834,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>712</v>
       </c>
@@ -4841,21 +4854,21 @@
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>381</v>
       </c>
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="93" t="s">
         <v>382</v>
       </c>
-      <c r="C22" s="92"/>
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
       <c r="F22" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>384</v>
       </c>
@@ -4875,21 +4888,21 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>385</v>
       </c>
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="93" t="s">
         <v>347</v>
       </c>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
       <c r="F24" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>390</v>
       </c>
@@ -4909,21 +4922,21 @@
         <v>391</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>387</v>
       </c>
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="93" t="s">
         <v>389</v>
       </c>
-      <c r="C26" s="92"/>
-      <c r="D26" s="92"/>
-      <c r="E26" s="92"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
       <c r="F26" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="81" t="s">
         <v>698</v>
       </c>
@@ -4938,7 +4951,7 @@
       </c>
       <c r="E27" s="80"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>405</v>
       </c>
@@ -4958,7 +4971,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>434</v>
       </c>
@@ -4978,7 +4991,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>410</v>
       </c>
@@ -5001,7 +5014,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>595</v>
       </c>
@@ -5024,7 +5037,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>579</v>
       </c>
@@ -5047,7 +5060,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>580</v>
       </c>
@@ -5070,16 +5083,16 @@
         <v>587</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>581</v>
       </c>
-      <c r="B34" s="93" t="s">
+      <c r="B34" s="94" t="s">
         <v>619</v>
       </c>
-      <c r="C34" s="93"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
       <c r="F34" t="s">
         <v>618</v>
       </c>
@@ -5087,7 +5100,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>469</v>
       </c>
@@ -5099,117 +5112,117 @@
         <v>470</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F49" s="70" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50" s="70" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51" s="70" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52" s="70" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53" s="70" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F54" s="70" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F56" s="70" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F57" s="70" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F58" s="70" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F59" s="70" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F60" s="70" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F61" s="70" t="s">
         <v>493</v>
       </c>
@@ -5240,42 +5253,42 @@
       <selection pane="bottomLeft" activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="5.81640625" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" customWidth="1"/>
-    <col min="10" max="10" width="5.7265625" customWidth="1"/>
-    <col min="11" max="11" width="5.453125" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" customWidth="1"/>
     <col min="12" max="12" width="5" customWidth="1"/>
-    <col min="13" max="17" width="5.453125" customWidth="1"/>
+    <col min="13" max="17" width="5.42578125" customWidth="1"/>
     <col min="18" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="5.26953125" customWidth="1"/>
-    <col min="20" max="21" width="5.453125" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" customWidth="1"/>
+    <col min="20" max="21" width="5.42578125" customWidth="1"/>
     <col min="22" max="22" width="4" customWidth="1"/>
-    <col min="23" max="23" width="4.54296875" customWidth="1"/>
-    <col min="24" max="25" width="3.81640625" customWidth="1"/>
-    <col min="26" max="28" width="5.453125" customWidth="1"/>
-    <col min="29" max="29" width="8.54296875" customWidth="1"/>
-    <col min="30" max="30" width="8.453125" customWidth="1"/>
+    <col min="23" max="23" width="4.5703125" customWidth="1"/>
+    <col min="24" max="25" width="3.85546875" customWidth="1"/>
+    <col min="26" max="28" width="5.42578125" customWidth="1"/>
+    <col min="29" max="29" width="8.5703125" customWidth="1"/>
+    <col min="30" max="30" width="8.42578125" customWidth="1"/>
     <col min="31" max="31" width="9" customWidth="1"/>
-    <col min="32" max="32" width="8.26953125" customWidth="1"/>
-    <col min="33" max="33" width="8.453125" customWidth="1"/>
-    <col min="34" max="35" width="8.26953125" customWidth="1"/>
-    <col min="36" max="36" width="9.1796875" customWidth="1"/>
-    <col min="37" max="38" width="9.1796875" style="84" customWidth="1"/>
-    <col min="39" max="42" width="9.1796875" style="87" customWidth="1"/>
-    <col min="45" max="45" width="8.81640625" customWidth="1"/>
-    <col min="46" max="46" width="13.1796875" customWidth="1"/>
+    <col min="32" max="32" width="8.28515625" customWidth="1"/>
+    <col min="33" max="33" width="8.42578125" customWidth="1"/>
+    <col min="34" max="35" width="8.28515625" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" customWidth="1"/>
+    <col min="37" max="38" width="9.140625" style="84" customWidth="1"/>
+    <col min="39" max="42" width="9.140625" style="87" customWidth="1"/>
+    <col min="45" max="45" width="8.85546875" customWidth="1"/>
+    <col min="46" max="46" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:48" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -5418,7 +5431,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>86</v>
       </c>
@@ -5545,7 +5558,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>87</v>
       </c>
@@ -5676,7 +5689,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>88</v>
       </c>
@@ -5801,7 +5814,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
@@ -5935,7 +5948,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>610</v>
       </c>
@@ -6082,7 +6095,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -6200,7 +6213,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -6324,7 +6337,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>611</v>
       </c>
@@ -6435,7 +6448,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>582</v>
       </c>
@@ -6543,7 +6556,7 @@
       </c>
       <c r="AQ10" s="87"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="T11" t="s">
         <v>679</v>
@@ -6562,7 +6575,7 @@
       </c>
       <c r="AQ11" s="87"/>
     </row>
-    <row r="12" spans="1:48" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:48" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>304</v>
       </c>
@@ -6598,7 +6611,7 @@
       <c r="AP12" s="85"/>
       <c r="AQ12" s="87"/>
     </row>
-    <row r="13" spans="1:48" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:48" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>86</v>
       </c>
@@ -6687,7 +6700,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="14" spans="1:48" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:48" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>87</v>
       </c>
@@ -6776,7 +6789,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="15" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>88</v>
       </c>
@@ -6865,7 +6878,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="16" spans="1:48" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:48" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>3</v>
       </c>
@@ -6946,7 +6959,7 @@
       </c>
       <c r="AJ16" s="88"/>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>305</v>
       </c>
@@ -7031,7 +7044,7 @@
       </c>
       <c r="AJ17" s="88"/>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>306</v>
       </c>
@@ -7116,7 +7129,7 @@
       </c>
       <c r="AJ18" s="88"/>
     </row>
-    <row r="19" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>307</v>
       </c>
@@ -7205,7 +7218,7 @@
       <c r="AN19" s="87"/>
       <c r="AO19" s="87"/>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>308</v>
       </c>
@@ -7274,7 +7287,7 @@
       </c>
       <c r="AJ20" s="88"/>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AC21" t="s">
         <v>5</v>
       </c>
@@ -7367,12 +7380,12 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -7383,7 +7396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -7394,7 +7407,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -7405,7 +7418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -7416,7 +7429,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -7424,7 +7437,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -7432,7 +7445,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>358</v>
       </c>
@@ -7440,22 +7453,22 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -7473,12 +7486,12 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="18.7265625" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>75</v>
       </c>
@@ -7522,7 +7535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -7572,7 +7585,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -7622,7 +7635,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -7672,7 +7685,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7719,7 +7732,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -7766,7 +7779,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7813,12 +7826,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="O9" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>75</v>
       </c>
@@ -7868,7 +7881,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -7916,7 +7929,7 @@
         <v>7400</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -7964,7 +7977,7 @@
         <v>8700</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -8012,7 +8025,7 @@
         <v>4900</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -8060,7 +8073,7 @@
         <v>6700</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -8101,7 +8114,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -8160,18 +8173,18 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.81640625" customWidth="1"/>
-    <col min="3" max="3" width="30.26953125" customWidth="1"/>
-    <col min="4" max="4" width="30.453125" customWidth="1"/>
-    <col min="5" max="5" width="35.26953125" customWidth="1"/>
-    <col min="6" max="6" width="19.54296875" customWidth="1"/>
-    <col min="7" max="7" width="34.54296875" customWidth="1"/>
-    <col min="8" max="8" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -8197,7 +8210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -8226,7 +8239,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -8255,7 +8268,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -8284,7 +8297,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -8313,7 +8326,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8342,7 +8355,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>324</v>
       </c>
@@ -8385,17 +8398,17 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="40.54296875" customWidth="1"/>
-    <col min="3" max="3" width="47.7265625" customWidth="1"/>
-    <col min="4" max="4" width="46.1796875" customWidth="1"/>
-    <col min="5" max="5" width="46.54296875" customWidth="1"/>
-    <col min="6" max="6" width="50.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" customWidth="1"/>
+    <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>196</v>
       </c>
@@ -8416,7 +8429,7 @@
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>175</v>
       </c>
@@ -8437,7 +8450,7 @@
       </c>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -8448,7 +8461,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>161</v>
       </c>
@@ -8469,7 +8482,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>5</v>
       </c>
@@ -8490,7 +8503,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>167</v>
       </c>
@@ -8511,7 +8524,7 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>165</v>
       </c>
@@ -8532,7 +8545,7 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>164</v>
       </c>
@@ -8553,7 +8566,7 @@
       </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>9</v>
       </c>
@@ -8564,7 +8577,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>166</v>
       </c>
@@ -8587,7 +8600,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>163</v>
       </c>
@@ -8610,7 +8623,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>162</v>
       </c>
@@ -8633,7 +8646,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>563</v>
       </c>
@@ -8654,7 +8667,7 @@
       </c>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>562</v>
       </c>
@@ -8675,7 +8688,7 @@
       </c>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>15</v>
       </c>
@@ -8686,7 +8699,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>542</v>
       </c>
@@ -8709,7 +8722,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>528</v>
       </c>
@@ -8732,7 +8745,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>529</v>
       </c>
@@ -8755,7 +8768,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>530</v>
       </c>
@@ -8778,7 +8791,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>531</v>
       </c>
@@ -8801,7 +8814,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>21</v>
       </c>
@@ -8824,7 +8837,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>546</v>
       </c>
@@ -8847,7 +8860,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>532</v>
       </c>
@@ -8870,7 +8883,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>533</v>
       </c>
@@ -8893,7 +8906,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>25</v>
       </c>
@@ -8916,7 +8929,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>26</v>
       </c>
@@ -8931,7 +8944,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>545</v>
       </c>
@@ -8954,7 +8967,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>534</v>
       </c>
@@ -8977,7 +8990,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>535</v>
       </c>
@@ -9000,7 +9013,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>536</v>
       </c>
@@ -9023,7 +9036,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>31</v>
       </c>
@@ -9046,7 +9059,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>544</v>
       </c>
@@ -9069,7 +9082,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="76" t="s">
         <v>527</v>
       </c>
@@ -9092,7 +9105,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="76" t="s">
         <v>537</v>
       </c>
@@ -9115,7 +9128,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>35</v>
       </c>
@@ -9138,7 +9151,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>36</v>
       </c>
@@ -9153,7 +9166,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>543</v>
       </c>
@@ -9176,7 +9189,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>538</v>
       </c>
@@ -9199,7 +9212,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>539</v>
       </c>
@@ -9222,7 +9235,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>540</v>
       </c>
@@ -9245,7 +9258,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>541</v>
       </c>
@@ -9268,7 +9281,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>42</v>
       </c>
@@ -9289,7 +9302,7 @@
       </c>
       <c r="G42" s="75"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>43</v>
       </c>
@@ -9307,7 +9320,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>44</v>
       </c>
@@ -9323,7 +9336,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>45</v>
       </c>
@@ -9339,7 +9352,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -9351,7 +9364,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -9363,7 +9376,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -9377,13 +9390,13 @@
         <v>642</v>
       </c>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49" s="77" t="s">
         <v>471</v>
       </c>
       <c r="G49" s="77"/>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E50" s="77" t="s">
         <v>472</v>
       </c>
@@ -9394,7 +9407,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51" s="77" t="s">
         <v>473</v>
       </c>
@@ -9405,7 +9418,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52" s="77" t="s">
         <v>474</v>
       </c>
@@ -9416,7 +9429,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53" s="77" t="s">
         <v>475</v>
       </c>
@@ -9427,7 +9440,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" s="77"/>
       <c r="F54" s="8" t="s">
         <v>480</v>
@@ -9436,7 +9449,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55" s="77" t="s">
         <v>476</v>
       </c>
@@ -9447,12 +9460,12 @@
         <v>648</v>
       </c>
     </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56" s="77" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57" s="77" t="s">
         <v>478</v>
       </c>
@@ -9463,7 +9476,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58" s="77" t="s">
         <v>479</v>
       </c>
@@ -9474,7 +9487,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59" s="77" t="s">
         <v>480</v>
       </c>
@@ -9485,7 +9498,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60" s="77" t="s">
         <v>481</v>
       </c>
@@ -9496,7 +9509,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
         <v>486</v>
       </c>
@@ -9504,7 +9517,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
         <v>487</v>
       </c>
@@ -9512,7 +9525,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="64" spans="5:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
         <v>488</v>
       </c>
@@ -9520,7 +9533,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="65" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
         <v>489</v>
       </c>
@@ -9528,7 +9541,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="66" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>658</v>
       </c>
@@ -9536,7 +9549,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="67" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
         <v>677</v>
       </c>
@@ -9544,7 +9557,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="68" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
         <v>492</v>
       </c>
@@ -9552,7 +9565,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="69" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
         <v>493</v>
       </c>
@@ -9568,38 +9581,38 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI40"/>
+  <dimension ref="A1:AI44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="4" width="7" customWidth="1"/>
-    <col min="5" max="7" width="8.7265625" customWidth="1"/>
-    <col min="8" max="8" width="8.1796875" customWidth="1"/>
-    <col min="9" max="9" width="6.81640625" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" customWidth="1"/>
-    <col min="13" max="13" width="8.1796875" customWidth="1"/>
-    <col min="14" max="14" width="6.7265625" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" customWidth="1"/>
-    <col min="17" max="17" width="6.7265625" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" customWidth="1"/>
-    <col min="19" max="19" width="8.54296875" customWidth="1"/>
-    <col min="20" max="20" width="7.1796875" customWidth="1"/>
-    <col min="21" max="21" width="9.54296875" customWidth="1"/>
-    <col min="22" max="22" width="8.453125" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" customWidth="1"/>
     <col min="23" max="23" width="8" customWidth="1"/>
     <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="26" width="13.1796875" customWidth="1"/>
-    <col min="27" max="27" width="8.26953125" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" customWidth="1"/>
+    <col min="27" max="27" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>196</v>
       </c>
@@ -9681,7 +9694,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>87</v>
       </c>
@@ -9780,7 +9793,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>88</v>
       </c>
@@ -9879,7 +9892,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>86</v>
       </c>
@@ -9978,7 +9991,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>202</v>
       </c>
@@ -10077,7 +10090,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>203</v>
       </c>
@@ -10171,7 +10184,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>205</v>
       </c>
@@ -10235,7 +10248,7 @@
         <v>1.439469444375E-2</v>
       </c>
       <c r="S7" s="7">
-        <f>SUM(S2:S5,S23:S40)</f>
+        <f>SUM(S2:S5,S27:S44)</f>
         <v>170603786000</v>
       </c>
       <c r="T7" s="32"/>
@@ -10244,7 +10257,7 @@
         <v>2.4764675484375002E-2</v>
       </c>
       <c r="V7" s="7">
-        <f>SUM(V2:V5,V23:V40)</f>
+        <f>SUM(V2:V5,V27:V44)</f>
         <v>293507265000</v>
       </c>
       <c r="W7" s="5"/>
@@ -10265,7 +10278,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -10303,7 +10316,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>3</v>
       </c>
@@ -10351,7 +10364,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
         <v>5</v>
       </c>
@@ -10393,7 +10406,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="26"/>
       <c r="D11" s="26"/>
@@ -10412,7 +10425,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -10463,7 +10476,7 @@
         <v>260000</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>211</v>
       </c>
@@ -10516,7 +10529,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>212</v>
       </c>
@@ -10569,7 +10582,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>213</v>
       </c>
@@ -10622,7 +10635,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -10675,7 +10688,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -10728,7 +10741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>216</v>
       </c>
@@ -10781,7 +10794,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>217</v>
       </c>
@@ -10834,44 +10847,44 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F20" s="50">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="G20" s="57">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="G20" s="53">
         <f>F20*H20</f>
-        <v>2880000000</v>
+        <v>816000000000</v>
       </c>
       <c r="H20">
-        <v>1800000000000</v>
+        <f>96*10^12</f>
+        <v>96000000000000</v>
       </c>
       <c r="T20" s="32"/>
       <c r="V20" s="32"/>
       <c r="W20" s="5"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F21" s="50">
-        <v>8.5000000000000006E-3</v>
-      </c>
-      <c r="G21" s="53">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="G21" s="57">
         <f>F21*H21</f>
-        <v>816000000000</v>
+        <v>2880000000</v>
       </c>
       <c r="H21">
-        <f>96*10^12</f>
-        <v>96000000000000</v>
+        <v>1800000000000</v>
       </c>
       <c r="T21" s="32"/>
       <c r="V21" s="32"/>
       <c r="W21" s="5"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>254</v>
       </c>
@@ -10892,201 +10905,65 @@
       <c r="V22" s="32"/>
       <c r="W22" s="5"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:26" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="92" t="s">
+        <v>723</v>
+      </c>
+      <c r="F23" s="50">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="G23" s="53">
+        <v>121318800000</v>
+      </c>
+      <c r="T23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="5"/>
+    </row>
+    <row r="24" spans="1:26" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="92" t="s">
+        <v>722</v>
+      </c>
+      <c r="F24" s="50">
+        <v>2.3E-3</v>
+      </c>
+      <c r="G24" s="53">
+        <v>37300000000</v>
+      </c>
+      <c r="T24" s="32"/>
+      <c r="V24" s="32"/>
+      <c r="W24" s="5"/>
+    </row>
+    <row r="25" spans="1:26" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="92" t="s">
+        <v>724</v>
+      </c>
+      <c r="F25" s="50">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="G25" s="53">
+        <v>165620000000</v>
+      </c>
+      <c r="T25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="5"/>
+    </row>
+    <row r="26" spans="1:26" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="92" t="s">
+        <v>725</v>
+      </c>
+      <c r="F26" s="50">
+        <v>2.18E-2</v>
+      </c>
+      <c r="G26" s="53">
+        <v>395000000000</v>
+      </c>
+      <c r="T26" s="32"/>
+      <c r="V26" s="32"/>
+      <c r="W26" s="5"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
         <v>218</v>
-      </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="27"/>
-      <c r="J23">
-        <v>11805300000</v>
-      </c>
-      <c r="K23" s="5">
-        <v>3.8989099999999999E-2</v>
-      </c>
-      <c r="L23" s="32"/>
-      <c r="M23">
-        <v>15207700000</v>
-      </c>
-      <c r="N23" s="5">
-        <v>3.8989099999999999E-2</v>
-      </c>
-      <c r="O23" s="32"/>
-      <c r="P23">
-        <v>28435000000</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>1.11854E-2</v>
-      </c>
-      <c r="S23">
-        <v>11053200000</v>
-      </c>
-      <c r="T23" s="32">
-        <v>3.8989099999999999E-2</v>
-      </c>
-      <c r="V23">
-        <v>22801100000</v>
-      </c>
-      <c r="W23" s="32">
-        <v>1.11854E-2</v>
-      </c>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A24" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
-      <c r="J24">
-        <v>10349200000</v>
-      </c>
-      <c r="K24" s="5">
-        <v>5.67772E-2</v>
-      </c>
-      <c r="L24" s="32"/>
-      <c r="M24">
-        <v>11929000000</v>
-      </c>
-      <c r="N24" s="5">
-        <v>5.67772E-2</v>
-      </c>
-      <c r="O24" s="32"/>
-      <c r="P24">
-        <v>18190100000</v>
-      </c>
-      <c r="Q24" s="5">
-        <v>2.07812E-2</v>
-      </c>
-      <c r="S24">
-        <v>9131780000</v>
-      </c>
-      <c r="T24" s="32">
-        <v>5.67772E-2</v>
-      </c>
-      <c r="V24">
-        <v>15002300000</v>
-      </c>
-      <c r="W24" s="32">
-        <v>2.07812E-2</v>
-      </c>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A25" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
-      <c r="J25">
-        <v>1854890000</v>
-      </c>
-      <c r="K25" s="5">
-        <v>9.5164600000000002E-2</v>
-      </c>
-      <c r="L25" s="32"/>
-      <c r="M25">
-        <v>2344760000</v>
-      </c>
-      <c r="N25" s="5">
-        <v>9.5164600000000002E-2</v>
-      </c>
-      <c r="O25" s="32"/>
-      <c r="P25">
-        <v>4234760000</v>
-      </c>
-      <c r="Q25" s="5">
-        <v>4.2202200000000002E-2</v>
-      </c>
-      <c r="S25">
-        <v>1717740000</v>
-      </c>
-      <c r="T25" s="32">
-        <v>9.5164600000000002E-2</v>
-      </c>
-      <c r="V25">
-        <v>3400310000</v>
-      </c>
-      <c r="W25" s="32">
-        <v>4.2202200000000002E-2</v>
-      </c>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A26" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="27"/>
-      <c r="J26">
-        <v>562322000</v>
-      </c>
-      <c r="K26" s="5">
-        <v>1.21885E-2</v>
-      </c>
-      <c r="L26" s="32"/>
-      <c r="M26">
-        <v>617912000</v>
-      </c>
-      <c r="N26" s="5">
-        <v>1.21885E-2</v>
-      </c>
-      <c r="O26" s="32"/>
-      <c r="P26">
-        <v>654576000</v>
-      </c>
-      <c r="Q26" s="5">
-        <v>4.6468000000000004E-3</v>
-      </c>
-      <c r="S26">
-        <v>504434000</v>
-      </c>
-      <c r="T26" s="32">
-        <v>1.21885E-2</v>
-      </c>
-      <c r="V26">
-        <v>607300000</v>
-      </c>
-      <c r="W26" s="32">
-        <v>4.6468000000000004E-3</v>
-      </c>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A27" s="23" t="s">
-        <v>222</v>
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="42"/>
@@ -11097,44 +10974,44 @@
       <c r="H27" s="26"/>
       <c r="I27" s="27"/>
       <c r="J27">
-        <v>1769430000</v>
+        <v>11805300000</v>
       </c>
       <c r="K27" s="5">
-        <v>2.4346699999999999E-2</v>
+        <v>3.8989099999999999E-2</v>
       </c>
       <c r="L27" s="32"/>
       <c r="M27">
-        <v>1687670000</v>
+        <v>15207700000</v>
       </c>
       <c r="N27" s="5">
-        <v>2.4346699999999999E-2</v>
+        <v>3.8989099999999999E-2</v>
       </c>
       <c r="O27" s="32"/>
       <c r="P27">
-        <v>1458560000</v>
+        <v>28435000000</v>
       </c>
       <c r="Q27" s="5">
-        <v>5.9619900000000003E-3</v>
+        <v>1.11854E-2</v>
       </c>
       <c r="S27">
-        <v>1490780000</v>
+        <v>11053200000</v>
       </c>
       <c r="T27" s="32">
-        <v>2.4346699999999999E-2</v>
+        <v>3.8989099999999999E-2</v>
       </c>
       <c r="V27">
-        <v>1433800000</v>
+        <v>22801100000</v>
       </c>
       <c r="W27" s="32">
-        <v>5.9619900000000003E-3</v>
+        <v>1.11854E-2</v>
       </c>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="42"/>
@@ -11145,44 +11022,44 @@
       <c r="H28" s="26"/>
       <c r="I28" s="27"/>
       <c r="J28">
-        <v>967764000</v>
+        <v>10349200000</v>
       </c>
       <c r="K28" s="5">
-        <v>2.92742E-3</v>
+        <v>5.67772E-2</v>
       </c>
       <c r="L28" s="32"/>
       <c r="M28">
-        <v>1179450000</v>
+        <v>11929000000</v>
       </c>
       <c r="N28" s="5">
-        <v>2.92742E-3</v>
+        <v>5.67772E-2</v>
       </c>
       <c r="O28" s="32"/>
       <c r="P28">
-        <v>1697440000</v>
+        <v>18190100000</v>
       </c>
       <c r="Q28" s="5">
-        <v>6.751950000000001E-5</v>
+        <v>2.07812E-2</v>
       </c>
       <c r="S28">
-        <v>902436999.99999988</v>
+        <v>9131780000</v>
       </c>
       <c r="T28" s="32">
-        <v>2.92742E-3</v>
+        <v>5.67772E-2</v>
       </c>
       <c r="V28">
-        <v>1432600000</v>
+        <v>15002300000</v>
       </c>
       <c r="W28" s="32">
-        <v>6.751950000000001E-5</v>
+        <v>2.07812E-2</v>
       </c>
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="42"/>
@@ -11193,44 +11070,44 @@
       <c r="H29" s="26"/>
       <c r="I29" s="27"/>
       <c r="J29">
-        <v>1044440000</v>
+        <v>1854890000</v>
       </c>
       <c r="K29" s="5">
-        <v>5.7337000000000004E-3</v>
+        <v>9.5164600000000002E-2</v>
       </c>
       <c r="L29" s="32"/>
       <c r="M29">
-        <v>1135210000</v>
+        <v>2344760000</v>
       </c>
       <c r="N29" s="5">
-        <v>5.7337000000000004E-3</v>
+        <v>9.5164600000000002E-2</v>
       </c>
       <c r="O29" s="32"/>
       <c r="P29">
-        <v>1171190000</v>
+        <v>4234760000</v>
       </c>
       <c r="Q29" s="5">
-        <v>2.7984199999999998E-3</v>
+        <v>4.2202200000000002E-2</v>
       </c>
       <c r="S29">
-        <v>910167000</v>
+        <v>1717740000</v>
       </c>
       <c r="T29" s="32">
-        <v>5.7337000000000004E-3</v>
+        <v>9.5164600000000002E-2</v>
       </c>
       <c r="V29">
-        <v>1086060000</v>
+        <v>3400310000</v>
       </c>
       <c r="W29" s="32">
-        <v>2.7984199999999998E-3</v>
+        <v>4.2202200000000002E-2</v>
       </c>
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
@@ -11241,44 +11118,44 @@
       <c r="H30" s="26"/>
       <c r="I30" s="27"/>
       <c r="J30">
-        <v>1152660000</v>
+        <v>562322000</v>
       </c>
       <c r="K30" s="5">
-        <v>4.7007999999999998E-3</v>
+        <v>1.21885E-2</v>
       </c>
       <c r="L30" s="32"/>
       <c r="M30">
-        <v>1027390000</v>
+        <v>617912000</v>
       </c>
       <c r="N30" s="5">
-        <v>4.7007999999999998E-3</v>
+        <v>1.21885E-2</v>
       </c>
       <c r="O30" s="32"/>
       <c r="P30">
-        <v>875014000</v>
+        <v>654576000</v>
       </c>
       <c r="Q30" s="5">
-        <v>1.9259699999999999E-3</v>
+        <v>4.6468000000000004E-3</v>
       </c>
       <c r="S30">
-        <v>918928000</v>
+        <v>504434000</v>
       </c>
       <c r="T30" s="32">
-        <v>4.7007999999999998E-3</v>
+        <v>1.21885E-2</v>
       </c>
       <c r="V30">
-        <v>834336000</v>
+        <v>607300000</v>
       </c>
       <c r="W30" s="32">
-        <v>1.9259699999999999E-3</v>
+        <v>4.6468000000000004E-3</v>
       </c>
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
@@ -11289,44 +11166,44 @@
       <c r="H31" s="26"/>
       <c r="I31" s="27"/>
       <c r="J31">
-        <v>3516000000</v>
+        <v>1769430000</v>
       </c>
       <c r="K31" s="5">
-        <v>7.9072999999999991E-2</v>
+        <v>2.4346699999999999E-2</v>
       </c>
       <c r="L31" s="32"/>
       <c r="M31">
-        <v>3731260000</v>
+        <v>1687670000</v>
       </c>
       <c r="N31" s="5">
-        <v>7.9072999999999991E-2</v>
+        <v>2.4346699999999999E-2</v>
       </c>
       <c r="O31" s="32"/>
       <c r="P31">
-        <v>3886050000</v>
+        <v>1458560000</v>
       </c>
       <c r="Q31" s="5">
-        <v>2.32768E-2</v>
+        <v>5.9619900000000003E-3</v>
       </c>
       <c r="S31">
-        <v>3020970000</v>
+        <v>1490780000</v>
       </c>
       <c r="T31" s="32">
-        <v>7.9072999999999991E-2</v>
+        <v>2.4346699999999999E-2</v>
       </c>
       <c r="V31">
-        <v>3561140000</v>
+        <v>1433800000</v>
       </c>
       <c r="W31" s="32">
-        <v>2.32768E-2</v>
+        <v>5.9619900000000003E-3</v>
       </c>
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="42"/>
@@ -11337,44 +11214,44 @@
       <c r="H32" s="26"/>
       <c r="I32" s="27"/>
       <c r="J32">
-        <v>441586000.00000012</v>
+        <v>967764000</v>
       </c>
       <c r="K32" s="5">
-        <v>9.5982800000000007E-3</v>
+        <v>2.92742E-3</v>
       </c>
       <c r="L32" s="32"/>
       <c r="M32">
-        <v>323198000</v>
+        <v>1179450000</v>
       </c>
       <c r="N32" s="5">
-        <v>9.5982800000000007E-3</v>
+        <v>2.92742E-3</v>
       </c>
       <c r="O32" s="32"/>
       <c r="P32">
-        <v>202741000</v>
+        <v>1697440000</v>
       </c>
       <c r="Q32" s="5">
-        <v>1.31111E-4</v>
+        <v>6.751950000000001E-5</v>
       </c>
       <c r="S32">
-        <v>321129000</v>
+        <v>902436999.99999988</v>
       </c>
       <c r="T32" s="32">
-        <v>9.5982800000000007E-3</v>
+        <v>2.92742E-3</v>
       </c>
       <c r="V32">
-        <v>202741000</v>
+        <v>1432600000</v>
       </c>
       <c r="W32" s="32">
-        <v>1.31111E-4</v>
+        <v>6.751950000000001E-5</v>
       </c>
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42"/>
@@ -11385,44 +11262,44 @@
       <c r="H33" s="26"/>
       <c r="I33" s="27"/>
       <c r="J33">
-        <v>2107760000</v>
+        <v>1044440000</v>
       </c>
       <c r="K33" s="5">
-        <v>0.234762</v>
+        <v>5.7337000000000004E-3</v>
       </c>
       <c r="L33" s="32"/>
       <c r="M33">
-        <v>2578780000</v>
+        <v>1135210000</v>
       </c>
       <c r="N33" s="5">
-        <v>0.234762</v>
+        <v>5.7337000000000004E-3</v>
       </c>
       <c r="O33" s="32"/>
       <c r="P33">
-        <v>4310250000</v>
+        <v>1171190000</v>
       </c>
       <c r="Q33" s="5">
-        <v>8.9194200000000001E-2</v>
+        <v>2.7984199999999998E-3</v>
       </c>
       <c r="S33">
-        <v>1896050000</v>
+        <v>910167000</v>
       </c>
       <c r="T33" s="32">
-        <v>0.234762</v>
+        <v>5.7337000000000004E-3</v>
       </c>
       <c r="V33">
-        <v>3457170000</v>
+        <v>1086060000</v>
       </c>
       <c r="W33" s="32">
-        <v>8.9194200000000001E-2</v>
+        <v>2.7984199999999998E-3</v>
       </c>
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="42"/>
@@ -11433,44 +11310,44 @@
       <c r="H34" s="26"/>
       <c r="I34" s="27"/>
       <c r="J34">
-        <v>68102200</v>
+        <v>1152660000</v>
       </c>
       <c r="K34" s="5">
-        <v>1.0055400000000001E-3</v>
+        <v>4.7007999999999998E-3</v>
       </c>
       <c r="L34" s="32"/>
       <c r="M34">
-        <v>56200000</v>
+        <v>1027390000</v>
       </c>
       <c r="N34" s="5">
-        <v>1.0055400000000001E-3</v>
+        <v>4.7007999999999998E-3</v>
       </c>
       <c r="O34" s="32"/>
       <c r="P34">
-        <v>46969300</v>
+        <v>875014000</v>
       </c>
       <c r="Q34" s="5">
-        <v>3.1115100000000002E-4</v>
+        <v>1.9259699999999999E-3</v>
       </c>
       <c r="S34">
-        <v>48499000</v>
+        <v>918928000</v>
       </c>
       <c r="T34" s="32">
-        <v>1.0055400000000001E-3</v>
+        <v>4.7007999999999998E-3</v>
       </c>
       <c r="V34">
-        <v>41783000</v>
+        <v>834336000</v>
       </c>
       <c r="W34" s="32">
-        <v>3.1115100000000002E-4</v>
+        <v>1.9259699999999999E-3</v>
       </c>
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="42"/>
@@ -11481,44 +11358,44 @@
       <c r="H35" s="26"/>
       <c r="I35" s="27"/>
       <c r="J35">
-        <v>625581000</v>
+        <v>3516000000</v>
       </c>
       <c r="K35" s="5">
-        <v>5.8450200000000001E-2</v>
+        <v>7.9072999999999991E-2</v>
       </c>
       <c r="L35" s="32"/>
       <c r="M35">
-        <v>781506000</v>
+        <v>3731260000</v>
       </c>
       <c r="N35" s="5">
-        <v>5.8450200000000001E-2</v>
+        <v>7.9072999999999991E-2</v>
       </c>
       <c r="O35" s="32"/>
       <c r="P35">
-        <v>980810999.99999988</v>
+        <v>3886050000</v>
       </c>
       <c r="Q35" s="5">
-        <v>2.76875E-2</v>
+        <v>2.32768E-2</v>
       </c>
       <c r="S35">
-        <v>576175000</v>
+        <v>3020970000</v>
       </c>
       <c r="T35" s="32">
-        <v>5.8450200000000001E-2</v>
+        <v>7.9072999999999991E-2</v>
       </c>
       <c r="V35">
-        <v>856456000</v>
+        <v>3561140000</v>
       </c>
       <c r="W35" s="32">
-        <v>2.76875E-2</v>
+        <v>2.32768E-2</v>
       </c>
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
@@ -11529,44 +11406,44 @@
       <c r="H36" s="26"/>
       <c r="I36" s="27"/>
       <c r="J36">
-        <v>8829090000</v>
+        <v>441586000.00000012</v>
       </c>
       <c r="K36" s="5">
-        <v>2.5381500000000001E-2</v>
+        <v>9.5982800000000007E-3</v>
       </c>
       <c r="L36" s="32"/>
       <c r="M36">
-        <v>10639300000</v>
+        <v>323198000</v>
       </c>
       <c r="N36" s="5">
-        <v>2.5381500000000001E-2</v>
+        <v>9.5982800000000007E-3</v>
       </c>
       <c r="O36" s="32"/>
       <c r="P36">
-        <v>17602700000</v>
+        <v>202741000</v>
       </c>
       <c r="Q36" s="5">
-        <v>8.5916800000000008E-3</v>
+        <v>1.31111E-4</v>
       </c>
       <c r="S36">
-        <v>7984630000</v>
+        <v>321129000</v>
       </c>
       <c r="T36" s="32">
-        <v>2.5381500000000001E-2</v>
+        <v>9.5982800000000007E-3</v>
       </c>
       <c r="V36">
-        <v>14344300000</v>
+        <v>202741000</v>
       </c>
       <c r="W36" s="32">
-        <v>8.5916800000000008E-3</v>
+        <v>1.31111E-4</v>
       </c>
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="42"/>
@@ -11577,44 +11454,44 @@
       <c r="H37" s="26"/>
       <c r="I37" s="27"/>
       <c r="J37">
-        <v>5884530000</v>
+        <v>2107760000</v>
       </c>
       <c r="K37" s="5">
-        <v>4.7133899999999996E-3</v>
+        <v>0.234762</v>
       </c>
       <c r="L37" s="32"/>
       <c r="M37">
-        <v>5229250000</v>
+        <v>2578780000</v>
       </c>
       <c r="N37" s="5">
-        <v>4.7133899999999996E-3</v>
+        <v>0.234762</v>
       </c>
       <c r="O37" s="32"/>
       <c r="P37">
-        <v>4093520000</v>
+        <v>4310250000</v>
       </c>
       <c r="Q37" s="5">
-        <v>1.4427299999999999E-3</v>
+        <v>8.9194200000000001E-2</v>
       </c>
       <c r="S37">
-        <v>4664430000</v>
+        <v>1896050000</v>
       </c>
       <c r="T37" s="32">
-        <v>4.7133899999999996E-3</v>
+        <v>0.234762</v>
       </c>
       <c r="V37">
-        <v>4051330000</v>
+        <v>3457170000</v>
       </c>
       <c r="W37" s="32">
-        <v>1.4427299999999999E-3</v>
+        <v>8.9194200000000001E-2</v>
       </c>
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="42"/>
@@ -11625,44 +11502,44 @@
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
       <c r="J38">
-        <v>2638440000</v>
+        <v>68102200</v>
       </c>
       <c r="K38" s="5">
-        <v>1.6438100000000001E-2</v>
+        <v>1.0055400000000001E-3</v>
       </c>
       <c r="L38" s="32"/>
       <c r="M38">
-        <v>3193060000</v>
+        <v>56200000</v>
       </c>
       <c r="N38" s="5">
-        <v>1.6438100000000001E-2</v>
+        <v>1.0055400000000001E-3</v>
       </c>
       <c r="O38" s="32"/>
       <c r="P38">
-        <v>5242770000</v>
+        <v>46969300</v>
       </c>
       <c r="Q38" s="5">
-        <v>5.8277199999999998E-3</v>
+        <v>3.1115100000000002E-4</v>
       </c>
       <c r="S38">
-        <v>2394240000</v>
+        <v>48499000</v>
       </c>
       <c r="T38" s="32">
-        <v>1.6438100000000001E-2</v>
+        <v>1.0055400000000001E-3</v>
       </c>
       <c r="V38">
-        <v>4273150000</v>
+        <v>41783000</v>
       </c>
       <c r="W38" s="32">
-        <v>5.8277199999999998E-3</v>
+        <v>3.1115100000000002E-4</v>
       </c>
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="42"/>
@@ -11673,44 +11550,44 @@
       <c r="H39" s="26"/>
       <c r="I39" s="27"/>
       <c r="J39">
-        <v>291907000</v>
+        <v>625581000</v>
       </c>
       <c r="K39" s="5">
-        <v>1.2645099999999999E-2</v>
+        <v>5.8450200000000001E-2</v>
       </c>
       <c r="L39" s="32"/>
       <c r="M39">
-        <v>316284000</v>
+        <v>781506000</v>
       </c>
       <c r="N39" s="5">
-        <v>1.2645099999999999E-2</v>
+        <v>5.8450200000000001E-2</v>
       </c>
       <c r="O39" s="32"/>
       <c r="P39">
-        <v>397545000</v>
+        <v>980810999.99999988</v>
       </c>
       <c r="Q39" s="5">
-        <v>4.0374499999999997E-3</v>
+        <v>2.76875E-2</v>
       </c>
       <c r="S39">
-        <v>250633000</v>
+        <v>576175000</v>
       </c>
       <c r="T39" s="32">
-        <v>1.2645099999999999E-2</v>
+        <v>5.8450200000000001E-2</v>
       </c>
       <c r="V39">
-        <v>339935000</v>
+        <v>856456000</v>
       </c>
       <c r="W39" s="32">
-        <v>4.0374499999999997E-3</v>
+        <v>2.76875E-2</v>
       </c>
       <c r="X39" s="5"/>
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="42"/>
@@ -11721,40 +11598,232 @@
       <c r="H40" s="26"/>
       <c r="I40" s="27"/>
       <c r="J40">
-        <v>823537999.99999988</v>
+        <v>8829090000</v>
       </c>
       <c r="K40" s="5">
-        <v>5.59604E-3</v>
+        <v>2.5381500000000001E-2</v>
       </c>
       <c r="L40" s="32"/>
       <c r="M40">
-        <v>710702000</v>
+        <v>10639300000</v>
       </c>
       <c r="N40" s="5">
-        <v>5.59604E-3</v>
+        <v>2.5381500000000001E-2</v>
       </c>
       <c r="O40" s="32"/>
       <c r="P40">
-        <v>539481000</v>
+        <v>17602700000</v>
       </c>
       <c r="Q40" s="5">
-        <v>1.08854E-3</v>
+        <v>8.5916800000000008E-3</v>
       </c>
       <c r="S40">
-        <v>650064000</v>
+        <v>7984630000</v>
       </c>
       <c r="T40" s="32">
-        <v>5.59604E-3</v>
+        <v>2.5381500000000001E-2</v>
       </c>
       <c r="V40">
-        <v>538354000</v>
+        <v>14344300000</v>
       </c>
       <c r="W40" s="32">
-        <v>1.08854E-3</v>
+        <v>8.5916800000000008E-3</v>
       </c>
       <c r="X40" s="5"/>
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="27"/>
+      <c r="J41">
+        <v>5884530000</v>
+      </c>
+      <c r="K41" s="5">
+        <v>4.7133899999999996E-3</v>
+      </c>
+      <c r="L41" s="32"/>
+      <c r="M41">
+        <v>5229250000</v>
+      </c>
+      <c r="N41" s="5">
+        <v>4.7133899999999996E-3</v>
+      </c>
+      <c r="O41" s="32"/>
+      <c r="P41">
+        <v>4093520000</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>1.4427299999999999E-3</v>
+      </c>
+      <c r="S41">
+        <v>4664430000</v>
+      </c>
+      <c r="T41" s="32">
+        <v>4.7133899999999996E-3</v>
+      </c>
+      <c r="V41">
+        <v>4051330000</v>
+      </c>
+      <c r="W41" s="32">
+        <v>1.4427299999999999E-3</v>
+      </c>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="27"/>
+      <c r="J42">
+        <v>2638440000</v>
+      </c>
+      <c r="K42" s="5">
+        <v>1.6438100000000001E-2</v>
+      </c>
+      <c r="L42" s="32"/>
+      <c r="M42">
+        <v>3193060000</v>
+      </c>
+      <c r="N42" s="5">
+        <v>1.6438100000000001E-2</v>
+      </c>
+      <c r="O42" s="32"/>
+      <c r="P42">
+        <v>5242770000</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>5.8277199999999998E-3</v>
+      </c>
+      <c r="S42">
+        <v>2394240000</v>
+      </c>
+      <c r="T42" s="32">
+        <v>1.6438100000000001E-2</v>
+      </c>
+      <c r="V42">
+        <v>4273150000</v>
+      </c>
+      <c r="W42" s="32">
+        <v>5.8277199999999998E-3</v>
+      </c>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="27"/>
+      <c r="J43">
+        <v>291907000</v>
+      </c>
+      <c r="K43" s="5">
+        <v>1.2645099999999999E-2</v>
+      </c>
+      <c r="L43" s="32"/>
+      <c r="M43">
+        <v>316284000</v>
+      </c>
+      <c r="N43" s="5">
+        <v>1.2645099999999999E-2</v>
+      </c>
+      <c r="O43" s="32"/>
+      <c r="P43">
+        <v>397545000</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>4.0374499999999997E-3</v>
+      </c>
+      <c r="S43">
+        <v>250633000</v>
+      </c>
+      <c r="T43" s="32">
+        <v>1.2645099999999999E-2</v>
+      </c>
+      <c r="V43">
+        <v>339935000</v>
+      </c>
+      <c r="W43" s="32">
+        <v>4.0374499999999997E-3</v>
+      </c>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="27"/>
+      <c r="J44">
+        <v>823537999.99999988</v>
+      </c>
+      <c r="K44" s="5">
+        <v>5.59604E-3</v>
+      </c>
+      <c r="L44" s="32"/>
+      <c r="M44">
+        <v>710702000</v>
+      </c>
+      <c r="N44" s="5">
+        <v>5.59604E-3</v>
+      </c>
+      <c r="O44" s="32"/>
+      <c r="P44">
+        <v>539481000</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>1.08854E-3</v>
+      </c>
+      <c r="S44">
+        <v>650064000</v>
+      </c>
+      <c r="T44" s="32">
+        <v>5.59604E-3</v>
+      </c>
+      <c r="V44">
+        <v>538354000</v>
+      </c>
+      <c r="W44" s="32">
+        <v>1.08854E-3</v>
+      </c>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11770,15 +11839,15 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="11.453125" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
     <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="33" max="33" width="11.453125" customWidth="1"/>
+    <col min="33" max="33" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="14" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="14" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -11877,7 +11946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -11988,7 +12057,7 @@
         <v>10.333402166480258</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -12097,7 +12166,7 @@
         <v>25.143552870628557</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -12206,7 +12275,7 @@
         <v>4.1054218110057965</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -12307,7 +12376,7 @@
         <v>3.9671629464069529</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -12411,7 +12480,7 @@
         <v>19.299485959819044</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -12514,7 +12583,7 @@
         <v>322.14084632849483</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -12573,7 +12642,7 @@
         <v>62.849025754340616</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -12632,7 +12701,7 @@
         <v>62.849025754340616</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -12644,7 +12713,7 @@
       </c>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -12657,7 +12726,7 @@
       </c>
       <c r="AB11" s="2"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -12722,7 +12791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>57</v>
       </c>
@@ -12736,7 +12805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>64</v>
       </c>
@@ -12744,7 +12813,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>72</v>
       </c>

</xml_diff>